<commit_message>
added more about food webs in space
</commit_message>
<xml_diff>
--- a/frameworks_foodwebs_in_space.xlsx
+++ b/frameworks_foodwebs_in_space.xlsx
@@ -19,183 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
-  <si>
-    <t>Advantages</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1996, 1999, 2002, 2009</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Years of important Papers</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Emergence of food web complexity</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Landscape theory of food web architecture and stability</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Metabolic theory, allometric scaling, consumer-resource models</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ecosystem dynamics</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Consumer-resource</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>People</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Frameworks</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Overarching Theory</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Focus</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Limitations</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Spatial Subsidies</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gary Polis, Wendy Anderson, Bob Holt</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bob Holt</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Trophic Island Biogeography</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Priyanga Amarasekare</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Food web complexity vs. type of movement</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kevin McCann</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stacked Specialist Food Chains</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">(1) mechanisms other than trophic rank (dependence) that may lead to predators being more sensitive to habitat size. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Assumptions</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Island Biogeography, Levins Metapopulations</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pradeep Pillai, Michel Loreau, Andrew Gonzalez</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Future Questions</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1) Do different mechanisms leads to different outcomes in metacommunity models?</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Model Types</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Patch dynamics</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1) spatially homogeneous envirionment, (2) global dispersal</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>consumer-resource, metacommunity</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1) does not incorporate spatial subsidies or energy flux from species outside the modules. (2) neglects 3-species food chains as a trophic module.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1) Setup different theoretical scenarios: specialist - generalist continnum is correlated with competition - colonization continuum and see how this influences food web assembly. (2) from a regional food web increase the colonization rate over a broad range and see if food web complexity is maximized at intermediate rates.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1) how does consumer foraging behavior (e.g. sit-and-wait vs. mobile, play into this framework?). (2) how does optimizing foraging time between birth and death rates influence consumer functional responses and therefore food web stability (see Abrams 1982)? (3) McCann - parasitoids will not tend to couple different energy pathways, although they may couple the same habitat type through behavioral (short range) and metacommunity dynamics (long range)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1) Decoupling two compartmentalized habitats from a shared top predator will destabilize both systems.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Integrative Questions &amp; Thoughts</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">(1) Would we still expect the same dynamics if we incorporate, say parasite/parasitoid body size relationships into these models? (2) How does the horizontal and vertical distribution of consumer functional responses influence food web stability? (3) Can we use these models to generate empirical predictions for how top-predator functional responses and differences in energy flux between pathways would affect stabilization/destabilization? </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1) hierarchical food web structure. (2) consumer behavior, instead of immigration/migration, couples spatially separated food webs.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Other Thoughts</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">(1) aggregates complex food webs into trophic groups. (2) assumptions do not conform to parasites/parasitoids having higher trophic position yet smaller body sizes. (3) ignores metacommunity dynamics. </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1) incorporates energy flux within and between food webs</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1) doesn't incorporate energy flux</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Major Outcomes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Food web complexity in metacommunities</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <r>
       <t xml:space="preserve">Succession &amp; Food webs: </t>
@@ -243,6 +67,186 @@
   </si>
   <si>
     <t>(1) incorporate arbitrarily large and complex food webs, (2) realistically characterizes how individual food web interactions occur.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patch dynamics</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) how does consumer foraging behavior (e.g. sit-and-wait vs. mobile, play into this framework?). (2) how does optimizing foraging time between birth and death rates influence consumer functional responses and therefore food web stability (see Abrams 1982)? (3) McCann - parasitoids will not tend to couple different energy pathways, although they may couple the same habitat type through behavioral (short range) and metacommunity dynamics (long range)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) Decoupling two compartmentalized habitats from a shared top predator will destabilize both systems.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integrative Questions &amp; Thoughts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) Would we still expect the same dynamics if we incorporate, say parasite/parasitoid body size relationships into these models? (2) How does the horizontal and vertical distribution of consumer functional responses influence food web stability? (3) Can we use these models to generate empirical predictions for how top-predator functional responses and differences in energy flux between pathways would affect stabilization/destabilization? </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) hierarchical food web structure. (2) consumer behavior, instead of immigration/migration, couples spatially separated food webs.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other Thoughts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) aggregates complex food webs into trophic groups. (2) assumptions do not conform to parasites/parasitoids having higher trophic position yet smaller body sizes. (3) ignores metacommunity dynamics. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) incorporates energy flux within and between food webs</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) doesn't incorporate energy flux</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Major Outcomes</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Food web complexity in metacommunities</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Advantages</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1996, 1999, 2002, 2009</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Years of important Papers</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Emergence of food web complexity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Landscape theory of food web architecture and stability</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Metabolic theory, allometric scaling, consumer-resource models</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ecosystem dynamics</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consumer-resource</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>People</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Frameworks</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overarching Theory</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Focus</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Limitations</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spatial Subsidies</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gary Polis, Wendy Anderson, Bob Holt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bob Holt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trophic Island Biogeography</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Priyanga Amarasekare</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Food web complexity vs. type of movement</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kevin McCann</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stacked Specialist Food Chains</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) mechanisms other than trophic rank (dependence) that may lead to predators being more sensitive to habitat size. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assumptions</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Island Biogeography, Levins Metapopulations</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pradeep Pillai, Michel Loreau, Andrew Gonzalez</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Future Questions</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) Do different mechanisms leads to different outcomes in metacommunity models?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Model Types</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Patch dynamics</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) spatially homogeneous envirionment, (2) global dispersal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>consumer-resource, metacommunity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) does not incorporate spatial subsidies or energy flux from species outside the modules. (2) neglects 3-species food chains as a trophic module.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1) Setup different theoretical scenarios: specialist - generalist continnum is correlated with competition - colonization continuum and see how this influences food web assembly. (2) from a regional food web increase the colonization rate over a broad range and see if food web complexity is maximized at intermediate rates.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -285,8 +289,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -630,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -649,191 +656,194 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="52">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1">
         <v>1997</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>44</v>
+        <v>5</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="52">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:14" ht="91">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:14" ht="130">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="M5" s="5"/>
       <c r="N5" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="65">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1">
         <v>2008</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>